<commit_message>
add stage flag to get_<xxx>_info.py, since authors and categories have different ids for production vs stage environments
</commit_message>
<xml_diff>
--- a/figleaf/figshare/researcher_metadata_figshare.xlsx
+++ b/figleaf/figshare/researcher_metadata_figshare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/figleaf/figleaf/figshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEF9534-7632-BB48-BC2A-DC21A7DDFA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC24DE2F-5642-5242-B987-1ACDC90033EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{F994D32C-DC09-7D4F-B37C-ED4B2EAE8784}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Virginia Scarlett</t>
   </si>
@@ -161,12 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,13 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F50D26F-5E03-AC45-84A4-9E66DD8565A6}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -527,8 +531,8 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
-        <v>14526911</v>
+      <c r="D3" s="1">
+        <v>2933718</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -553,66 +557,66 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>9314359</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D9" s="1">
+        <v>25718</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,10 +627,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4">
-        <v>24748</v>
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
+        <v>310112</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,13 +638,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>320999</v>
+        <v>26104</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -651,37 +655,23 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
-        <v>24169</v>
+        <v>320999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2</v>
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1">
-        <v>310112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add another author with rich author metadata to spreadsheet
</commit_message>
<xml_diff>
--- a/figleaf/figshare/researcher_metadata_figshare.xlsx
+++ b/figleaf/figshare/researcher_metadata_figshare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/figleaf/figleaf/figshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC24DE2F-5642-5242-B987-1ACDC90033EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DDE34C-9434-7E49-ACF0-8B8E3D8CBC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{F994D32C-DC09-7D4F-B37C-ED4B2EAE8784}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Virginia Scarlett</t>
   </si>
@@ -65,9 +65,6 @@
     <t>authors</t>
   </si>
   <si>
-    <t>url_name</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -95,17 +92,41 @@
     <t>name</t>
   </si>
   <si>
-    <t>Ana_Van_Gulick</t>
-  </si>
-  <si>
     <t>Ana Van Gulick</t>
+  </si>
+  <si>
+    <t>William Shakespeare</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>Shakespeare</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>thebard@hotmail.com</t>
+  </si>
+  <si>
+    <t>orcid_id</t>
+  </si>
+  <si>
+    <t>000-000-12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +161,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,8 +187,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -167,9 +197,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,16 +513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F50D26F-5E03-AC45-84A4-9E66DD8565A6}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="10.83203125" style="5"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -515,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -543,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -554,128 +582,187 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <v>25718</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1">
-        <v>310112</v>
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1">
-        <v>26104</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1">
+        <v>25718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1">
+        <v>310112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1">
+        <v>26104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1">
+        <v>320999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1">
-        <v>320999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{51DA04AB-3EEB-4846-94EF-3411AEA3A9F2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove orcid_id from spreadsheet
</commit_message>
<xml_diff>
--- a/figleaf/figshare/researcher_metadata_figshare.xlsx
+++ b/figleaf/figshare/researcher_metadata_figshare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/figleaf/figleaf/figshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DDE34C-9434-7E49-ACF0-8B8E3D8CBC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405DE197-5930-364B-8112-5EDCD57FB5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{F994D32C-DC09-7D4F-B37C-ED4B2EAE8784}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Virginia Scarlett</t>
   </si>
@@ -114,12 +114,6 @@
   </si>
   <si>
     <t>thebard@hotmail.com</t>
-  </si>
-  <si>
-    <t>orcid_id</t>
-  </si>
-  <si>
-    <t>000-000-12345</t>
   </si>
 </sst>
 </file>
@@ -516,7 +510,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,13 +576,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>650798</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -599,10 +593,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -613,10 +607,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -627,10 +621,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,10 +635,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -761,7 +755,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{51DA04AB-3EEB-4846-94EF-3411AEA3A9F2}"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{51DA04AB-3EEB-4846-94EF-3411AEA3A9F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>